<commit_message>
This is my Third day first commit.
</commit_message>
<xml_diff>
--- a/LOPAMUDRA_BERA.xlsx
+++ b/LOPAMUDRA_BERA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="125">
   <si>
     <t>S.No</t>
   </si>
@@ -321,6 +321,118 @@
   </si>
   <si>
     <t>90Minutes</t>
+  </si>
+  <si>
+    <t>Understanding the DAO pattern.</t>
+  </si>
+  <si>
+    <t>Self Study of DAO</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=9fVQ_mvzV48</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=H1mePFyqqiE</t>
+  </si>
+  <si>
+    <t>40Minutes</t>
+  </si>
+  <si>
+    <t>Mock</t>
+  </si>
+  <si>
+    <t>20Minutes</t>
+  </si>
+  <si>
+    <t>https://www.codeproject.com/Articles/93369/How-I-explained-OOD-to-my-wife</t>
+  </si>
+  <si>
+    <t>Create model class Product with the following parameters(ID, Brand, Name, Description, Price, Quantity, Category, Supplier). Similarly create for Category and User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=F2L24Cy4zkQ, </t>
+  </si>
+  <si>
+    <t>Linking DAO with Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement DAO Pattern </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=STi8nP7yArs</t>
+  </si>
+  <si>
+    <t>JSTL core tag in not allowed in tomcat eclipse</t>
+  </si>
+  <si>
+    <t>Lopa_ERR3</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Add dependenct inside pom.xml file:"&lt;dependency&gt;
+&lt;groupId&gt;jstl&lt;/groupId&gt;
+&lt;artifactId&gt;jstl&lt;/artifactId&gt;
+&lt;version&gt;1.2&lt;/version&gt;
+&lt;/dependency&gt;"</t>
+  </si>
+  <si>
+    <t>List as datasource for table in products page</t>
+  </si>
+  <si>
+    <t>Lopa_ERR4</t>
+  </si>
+  <si>
+    <t>Route to a Products Page from the productDetail page on clicking on a button which will show the details of the product for which more info is required.</t>
+  </si>
+  <si>
+    <t>Image is not diplaying on allproduct page</t>
+  </si>
+  <si>
+    <t>In ProductDAOImpl file passed only image name with extension and in productDetail.jsp page src value as ${images}/${product.imageUrl}</t>
+  </si>
+  <si>
+    <t>Lopa_ERR3, Lopa_ERR4</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/com.fasterxml.jackson.core/jackson-databind/2.2.3</t>
+  </si>
+  <si>
+    <t>Lopa_ERR5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Failure to add jackson dependency. Due to multiple attempt for poor network cache was fool for re-attempt. </t>
+  </si>
+  <si>
+    <t>Open physical path of the maven in machine i.e. C:\Users\LOPA B\.m2\repository\com\, and delete fasterxml folder. Then go back to Eclipse and refresh.</t>
+  </si>
+  <si>
+    <t>datatable</t>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/18441629/noclassdeffounderror-com-fasterxml-jackson-core-treenode-json-schema-validati</t>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/8886614/uncaught-referenceerror-jquery-is-not-defined</t>
+  </si>
+  <si>
+    <t>Uncaught jquery exception</t>
+  </si>
+  <si>
+    <t>jquery script must be added first and then bootstrap</t>
+  </si>
+  <si>
+    <t>Lopa_ERR6</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Lopa_ERR5, Lopa_ERR6</t>
+  </si>
+  <si>
+    <t>3hrs</t>
   </si>
 </sst>
 </file>
@@ -385,7 +497,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -432,6 +544,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -441,7 +562,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -512,6 +633,54 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -795,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1316,14 +1485,262 @@
         <v>20</v>
       </c>
     </row>
+    <row r="22" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="34">
+        <v>42795</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="44"/>
+      <c r="E22" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
+        <v>22</v>
+      </c>
+      <c r="B23" s="34">
+        <v>42795</v>
+      </c>
+      <c r="C23" s="43"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="47"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="47"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>23</v>
+      </c>
+      <c r="B24" s="34">
+        <v>42795</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="38"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G24" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
+      <c r="B25" s="34">
+        <v>42795</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="38"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
+      <c r="B26" s="34">
+        <v>42795</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
+        <v>26</v>
+      </c>
+      <c r="B27" s="34">
+        <v>42795</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>27</v>
+      </c>
+      <c r="B28" s="34">
+        <v>42795</v>
+      </c>
+      <c r="C28" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28" s="39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
+        <v>28</v>
+      </c>
+      <c r="B29" s="34">
+        <v>42795</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>29</v>
+      </c>
+      <c r="B30" s="34">
+        <v>42795</v>
+      </c>
+      <c r="C30" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
+        <v>30</v>
+      </c>
+      <c r="B31" s="34"/>
+      <c r="C31" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="E31" s="41"/>
+      <c r="F31" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H31" s="48" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>31</v>
+      </c>
+      <c r="B32" s="34">
+        <v>42795</v>
+      </c>
+      <c r="C32" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" display="http://www.techrepublic.com/blog/it-consultant/define-project-scope-to-include-deliverables-boundaries-and-requirements"/>
     <hyperlink ref="D7" r:id="rId2" display="https://www.youtube.com/watch?v=FOtx1lO9SS4"/>
     <hyperlink ref="D8" r:id="rId3" display="https://www.youtube.com/watch?v=pU-4NybcjnE&amp;list=PLBgMUB7xGcO1YY1J9NoXssmaB0FjLSbQ5"/>
+    <hyperlink ref="E22" r:id="rId4"/>
+    <hyperlink ref="E23" r:id="rId5"/>
+    <hyperlink ref="E28" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1332,7 +1749,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1384,23 +1801,55 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+    <row r="4" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="41"/>
     </row>
     <row r="5" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="3"/>
+      <c r="A5" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>110</v>
+      </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>115</v>
+      </c>
       <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>

</xml_diff>

<commit_message>
This is my Fourth day first commit.
</commit_message>
<xml_diff>
--- a/LOPAMUDRA_BERA.xlsx
+++ b/LOPAMUDRA_BERA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="145">
   <si>
     <t>S.No</t>
   </si>
@@ -433,6 +433,70 @@
   </si>
   <si>
     <t>3hrs</t>
+  </si>
+  <si>
+    <t>Adding Dependencies for implementing Spring Hibernate ORM with H2 Database</t>
+  </si>
+  <si>
+    <t>adding applicationContext.xml and connect it using web.xml</t>
+  </si>
+  <si>
+    <t>Create Beans for DataSource, SessionFactory, TransactionManager in applicationContext.xml file. After successful configuration, a table Product should get created in H2 database.</t>
+  </si>
+  <si>
+    <t>Put some sample data in the table and it should be retrieved in the Products Page in the datatable.</t>
+  </si>
+  <si>
+    <t>Write the Junit test cases for checking the DAO classes</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com</t>
+  </si>
+  <si>
+    <t>4hrs</t>
+  </si>
+  <si>
+    <t>Lopa_ERR7</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.hibernate/ejb3-persistence</t>
+  </si>
+  <si>
+    <t>Lopa_ERR8</t>
+  </si>
+  <si>
+    <t>&lt;dependency&gt;
+      &lt;groupId&gt;org.hibernate&lt;/groupId&gt;
+      &lt;artifactId&gt;ejb3-persistence&lt;/artifactId&gt;
+      &lt;version&gt;1.0&lt;/version&gt;
+  &lt;/dependency&gt;</t>
+  </si>
+  <si>
+    <t>Not regognised @Entity annotation</t>
+  </si>
+  <si>
+    <t>1hrs</t>
+  </si>
+  <si>
+    <t>1hr</t>
+  </si>
+  <si>
+    <t>Lopa_ERR9</t>
+  </si>
+  <si>
+    <t>Unable to create table to database</t>
+  </si>
+  <si>
+    <t>Changed database and user name</t>
+  </si>
+  <si>
+    <t>Unable to found dependency jars of hibernate, commons-dbcp etc.</t>
+  </si>
+  <si>
+    <t>Go to Maven Build Path&gt;&gt;libraries and add jdk1.8 instead of jre.</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -661,6 +725,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -677,9 +744,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -964,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1492,20 +1556,20 @@
       <c r="B22" s="34">
         <v>42795</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="44"/>
+      <c r="D22" s="45"/>
       <c r="E22" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="46" t="s">
+      <c r="F22" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="46" t="s">
+      <c r="G22" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="47" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1516,14 +1580,14 @@
       <c r="B23" s="34">
         <v>42795</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="45"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="46"/>
       <c r="E23" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="47"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="47"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="48"/>
     </row>
     <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
@@ -1696,7 +1760,7 @@
       <c r="G31" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H31" s="48" t="s">
+      <c r="H31" s="42" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1722,6 +1786,114 @@
       <c r="G32" s="1" t="s">
         <v>122</v>
       </c>
+    </row>
+    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>32</v>
+      </c>
+      <c r="B33" s="28">
+        <v>42796</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>33</v>
+      </c>
+      <c r="B34" s="28">
+        <v>42796</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>34</v>
+      </c>
+      <c r="B35" s="28">
+        <v>42796</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>35</v>
+      </c>
+      <c r="B36" s="28">
+        <v>42796</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>36</v>
+      </c>
+      <c r="B37" s="28">
+        <v>42796</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1746,17 +1918,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A4" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.109375" customWidth="1"/>
     <col min="2" max="2" width="106.109375" customWidth="1"/>
-    <col min="3" max="3" width="52.33203125" customWidth="1"/>
+    <col min="3" max="3" width="54.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="56.44140625" customWidth="1"/>
     <col min="5" max="10" width="9.109375" customWidth="1"/>
   </cols>
@@ -1852,13 +2024,49 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="D8" s="14"/>
-    </row>
-    <row r="9" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="A8" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="30"/>
+    </row>
+    <row r="9" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>